<commit_message>
Updated simpleNMR.py Added create new nmr problem from mnova data by copy pasting Added some new example problems Added a save menu that saves the xy3 data to the nmrproblem directory Added an open menu item to open a new nmr problem directory
</commit_message>
<xml_diff>
--- a/exampleProblems/ch9_069/ch9_069.xlsx
+++ b/exampleProblems/ch9_069/ch9_069.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://durhamuniversity-my.sharepoint.com/personal/vsmw51_durham_ac_uk/Documents/projects/programming/2022/python/python/rdkit37/projects/simpleNMR/exampleProblems/ch9_069/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="264" documentId="11_9DFAB9B766D6D4A00340053428BA5669BEDDD768" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D9B342B7-C751-470E-B3D7-3E513894340A}"/>
+  <xr:revisionPtr revIDLastSave="302" documentId="11_9DFAB9B766D6D4A00340053428BA5669BEDDD768" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ED7F16B4-2599-4A21-8BBF-80E5EC2097DC}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7185" yWindow="780" windowWidth="20295" windowHeight="13620" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="molecule" sheetId="9" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="48">
   <si>
     <t>Name</t>
   </si>
@@ -123,9 +123,6 @@
     <t>3.37 .. 2.29</t>
   </si>
   <si>
-    <t>2.09 .. 2.01</t>
-  </si>
-  <si>
     <t>2.04 .. 1.96</t>
   </si>
   <si>
@@ -175,6 +172,9 @@
   </si>
   <si>
     <t>8,7,6, 6</t>
+  </si>
+  <si>
+    <t>2.14 .. 2.06</t>
   </si>
 </sst>
 </file>
@@ -611,8 +611,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -660,7 +660,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C2" s="1">
         <v>4.12</v>
@@ -675,10 +675,10 @@
         <v>1</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I2" t="s">
         <v>8</v>
@@ -689,7 +689,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C3" s="1">
         <v>3.4</v>
@@ -704,10 +704,10 @@
         <v>1</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="I3" t="s">
         <v>8</v>
@@ -718,7 +718,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C4" s="1">
         <v>3.32</v>
@@ -733,10 +733,10 @@
         <v>1</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I4" t="s">
         <v>8</v>
@@ -747,7 +747,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C5" s="1">
         <v>2.33</v>
@@ -762,10 +762,10 @@
         <v>1</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="I5" t="s">
         <v>8</v>
@@ -776,13 +776,13 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C6" s="1">
-        <v>2.0499999999999998</v>
+        <v>2.1</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>30</v>
+        <v>47</v>
       </c>
       <c r="E6" s="1">
         <v>1</v>
@@ -791,10 +791,10 @@
         <v>1</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="I6" t="s">
         <v>8</v>
@@ -805,13 +805,13 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C7" s="1">
         <v>2</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E7" s="1">
         <v>2</v>
@@ -820,10 +820,10 @@
         <v>2</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I7" t="s">
         <v>8</v>
@@ -870,7 +870,7 @@
   <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1037,7 +1037,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1">
-        <v>2.0499999999999998</v>
+        <v>2.1</v>
       </c>
       <c r="C6" s="1">
         <v>31.7</v>
@@ -1063,7 +1063,9 @@
       <c r="J6" s="1"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
+      <c r="A7" s="5">
+        <v>6</v>
+      </c>
       <c r="B7" s="1">
         <v>2</v>
       </c>
@@ -1144,10 +1146,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:T35"/>
+  <dimension ref="A1:T31"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1:L20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1201,19 +1203,19 @@
         <v>4.12</v>
       </c>
       <c r="C2" s="1">
-        <v>4.12</v>
+        <v>2.33</v>
       </c>
       <c r="D2" s="1">
         <v>1</v>
       </c>
       <c r="E2" s="1">
-        <v>6.29</v>
+        <v>1</v>
       </c>
       <c r="F2" s="1">
-        <v>27.7</v>
+        <v>1</v>
       </c>
       <c r="G2" s="1">
-        <v>24.96</v>
+        <v>1</v>
       </c>
       <c r="H2" s="1" t="s">
         <v>17</v>
@@ -1227,22 +1229,22 @@
         <v>2</v>
       </c>
       <c r="B3" s="1">
-        <v>3.4</v>
+        <v>4.12</v>
       </c>
       <c r="C3" s="1">
-        <v>3.4</v>
+        <v>2.1</v>
       </c>
       <c r="D3" s="1">
-        <v>1.6</v>
+        <v>1</v>
       </c>
       <c r="E3" s="1">
-        <v>5.74</v>
+        <v>1</v>
       </c>
       <c r="F3" s="1">
-        <v>40.520000000000003</v>
+        <v>1</v>
       </c>
       <c r="G3" s="1">
-        <v>49.97</v>
+        <v>1</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>17</v>
@@ -1256,22 +1258,22 @@
         <v>3</v>
       </c>
       <c r="B4" s="1">
-        <v>3.32</v>
+        <v>2.1</v>
       </c>
       <c r="C4" s="1">
-        <v>3.32</v>
+        <v>2</v>
       </c>
       <c r="D4" s="1">
-        <v>1.8</v>
+        <v>1</v>
       </c>
       <c r="E4" s="1">
-        <v>4.51</v>
+        <v>1</v>
       </c>
       <c r="F4" s="1">
-        <v>26.61</v>
+        <v>1</v>
       </c>
       <c r="G4" s="1">
-        <v>28.84</v>
+        <v>1</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>17</v>
@@ -1288,19 +1290,19 @@
         <v>2.33</v>
       </c>
       <c r="C5" s="1">
-        <v>2.33</v>
+        <v>2</v>
       </c>
       <c r="D5" s="1">
-        <v>0.4</v>
+        <v>1</v>
       </c>
       <c r="E5" s="1">
-        <v>4.6399999999999997</v>
+        <v>1</v>
       </c>
       <c r="F5" s="1">
-        <v>16.96</v>
+        <v>1</v>
       </c>
       <c r="G5" s="1">
-        <v>4.3099999999999996</v>
+        <v>1</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>17</v>
@@ -1314,22 +1316,22 @@
         <v>5</v>
       </c>
       <c r="B6" s="1">
-        <v>2.0499999999999998</v>
+        <v>2</v>
       </c>
       <c r="C6" s="1">
-        <v>2.0499999999999998</v>
+        <v>3.4</v>
       </c>
       <c r="D6" s="1">
-        <v>1.1000000000000001</v>
+        <v>1</v>
       </c>
       <c r="E6" s="1">
-        <v>5.97</v>
+        <v>1</v>
       </c>
       <c r="F6" s="1">
-        <v>31.34</v>
+        <v>1</v>
       </c>
       <c r="G6" s="1">
-        <v>27.49</v>
+        <v>1</v>
       </c>
       <c r="H6" s="1" t="s">
         <v>17</v>
@@ -1339,381 +1341,92 @@
       </c>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A7" s="5">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1">
-        <v>2</v>
-      </c>
-      <c r="C7" s="1">
-        <v>2</v>
-      </c>
-      <c r="D7" s="1">
-        <v>1</v>
-      </c>
-      <c r="E7" s="1">
-        <v>1</v>
-      </c>
-      <c r="F7" s="1">
-        <v>1</v>
-      </c>
-      <c r="G7" s="1">
-        <v>1</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I7" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A8" s="5">
-        <v>7</v>
-      </c>
-      <c r="B8" s="1">
-        <v>4.12</v>
-      </c>
-      <c r="C8" s="1">
-        <v>2.33</v>
-      </c>
-      <c r="D8" s="1">
-        <v>1</v>
-      </c>
-      <c r="E8" s="1">
-        <v>1</v>
-      </c>
-      <c r="F8" s="1">
-        <v>1</v>
-      </c>
-      <c r="G8" s="1">
-        <v>1</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A9" s="5">
-        <v>8</v>
-      </c>
-      <c r="B9" s="1">
-        <v>2.33</v>
-      </c>
-      <c r="C9" s="1">
-        <v>4.12</v>
-      </c>
-      <c r="D9" s="1">
-        <v>1</v>
-      </c>
-      <c r="E9" s="1">
-        <v>1</v>
-      </c>
-      <c r="F9" s="1">
-        <v>1</v>
-      </c>
-      <c r="G9" s="1">
-        <v>1</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A10" s="5">
-        <v>9</v>
-      </c>
-      <c r="B10" s="1">
-        <v>4.12</v>
-      </c>
-      <c r="C10" s="1">
-        <v>2.0499999999999998</v>
-      </c>
-      <c r="D10" s="1">
-        <v>1</v>
-      </c>
-      <c r="E10" s="1">
-        <v>1</v>
-      </c>
-      <c r="F10" s="1">
-        <v>1</v>
-      </c>
-      <c r="G10" s="1">
-        <v>1</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A11" s="5">
-        <v>10</v>
-      </c>
-      <c r="B11" s="1">
-        <v>2.0499999999999998</v>
-      </c>
-      <c r="C11" s="1">
-        <v>4.12</v>
-      </c>
-      <c r="D11" s="1">
-        <v>1</v>
-      </c>
-      <c r="E11" s="1">
-        <v>1</v>
-      </c>
-      <c r="F11" s="1">
-        <v>1</v>
-      </c>
-      <c r="G11" s="1">
-        <v>1</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A12" s="5">
-        <v>11</v>
-      </c>
-      <c r="B12" s="1">
-        <v>2.0499999999999998</v>
-      </c>
-      <c r="C12" s="1">
-        <v>2</v>
-      </c>
-      <c r="D12" s="1">
-        <v>1</v>
-      </c>
-      <c r="E12" s="1">
-        <v>1</v>
-      </c>
-      <c r="F12" s="1">
-        <v>1</v>
-      </c>
-      <c r="G12" s="1">
-        <v>1</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>18</v>
-      </c>
+      <c r="A7" s="5"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A13" s="5">
-        <v>12</v>
-      </c>
-      <c r="B13" s="1">
-        <v>2</v>
-      </c>
-      <c r="C13" s="1">
-        <v>2.0499999999999998</v>
-      </c>
-      <c r="D13" s="1">
-        <v>1</v>
-      </c>
-      <c r="E13" s="1">
-        <v>1</v>
-      </c>
-      <c r="F13" s="1">
-        <v>1</v>
-      </c>
-      <c r="G13" s="1">
-        <v>1</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>18</v>
-      </c>
+      <c r="A13" s="5"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A14" s="5">
-        <v>13</v>
-      </c>
-      <c r="B14" s="1">
-        <v>2.33</v>
-      </c>
-      <c r="C14" s="1">
-        <v>2</v>
-      </c>
-      <c r="D14" s="1">
-        <v>1</v>
-      </c>
-      <c r="E14" s="1">
-        <v>1</v>
-      </c>
-      <c r="F14" s="1">
-        <v>1</v>
-      </c>
-      <c r="G14" s="1">
-        <v>1</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I14" s="1" t="s">
-        <v>18</v>
-      </c>
+      <c r="A14" s="5"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
     </row>
     <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A15" s="5">
-        <v>14</v>
-      </c>
-      <c r="B15" s="1">
-        <v>2</v>
-      </c>
-      <c r="C15" s="1">
-        <v>2.33</v>
-      </c>
-      <c r="D15" s="1">
-        <v>1</v>
-      </c>
-      <c r="E15" s="1">
-        <v>1</v>
-      </c>
-      <c r="F15" s="1">
-        <v>1</v>
-      </c>
-      <c r="G15" s="1">
-        <v>1</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>18</v>
-      </c>
+      <c r="A15" s="5"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
     </row>
     <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A16" s="5">
-        <v>15</v>
-      </c>
-      <c r="B16" s="1">
-        <v>2</v>
-      </c>
-      <c r="C16" s="1">
-        <v>3.4</v>
-      </c>
-      <c r="D16" s="1">
-        <v>1</v>
-      </c>
-      <c r="E16" s="1">
-        <v>1</v>
-      </c>
-      <c r="F16" s="1">
-        <v>1</v>
-      </c>
-      <c r="G16" s="1">
-        <v>1</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>18</v>
-      </c>
+      <c r="A16" s="5"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="5">
-        <v>16</v>
-      </c>
-      <c r="B17" s="1">
-        <v>3.4</v>
-      </c>
-      <c r="C17" s="1">
-        <v>2</v>
-      </c>
-      <c r="D17" s="1">
-        <v>1</v>
-      </c>
-      <c r="E17" s="1">
-        <v>1</v>
-      </c>
-      <c r="F17" s="1">
-        <v>1</v>
-      </c>
-      <c r="G17" s="1">
-        <v>1</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>18</v>
-      </c>
+      <c r="A17" s="5"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="1"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="5">
-        <v>17</v>
-      </c>
-      <c r="B18" s="1">
-        <v>2</v>
-      </c>
-      <c r="C18" s="1">
-        <v>3.32</v>
-      </c>
-      <c r="D18" s="1">
-        <v>1</v>
-      </c>
-      <c r="E18" s="1">
-        <v>1</v>
-      </c>
-      <c r="F18" s="1">
-        <v>1</v>
-      </c>
-      <c r="G18" s="1">
-        <v>1</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>18</v>
-      </c>
+      <c r="A18" s="5"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="5">
-        <v>18</v>
-      </c>
-      <c r="B19" s="1">
-        <v>3.32</v>
-      </c>
-      <c r="C19" s="1">
-        <v>2</v>
-      </c>
-      <c r="D19" s="1">
-        <v>1</v>
-      </c>
-      <c r="E19" s="1">
-        <v>1</v>
-      </c>
-      <c r="F19" s="1">
-        <v>1</v>
-      </c>
-      <c r="G19" s="1">
-        <v>1</v>
-      </c>
-      <c r="H19" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>18</v>
-      </c>
+      <c r="A19" s="5"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="1"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="5"/>
@@ -1815,15 +1528,15 @@
       <c r="I28" s="1"/>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="5"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
-      <c r="H29" s="1"/>
-      <c r="I29" s="1"/>
+      <c r="A29" s="6"/>
+      <c r="B29" s="7"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="7"/>
+      <c r="I29" s="7"/>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" s="5"/>
@@ -1837,59 +1550,15 @@
       <c r="I30" s="1"/>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A31" s="5"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
-      <c r="H31" s="1"/>
-      <c r="I31" s="1"/>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A32" s="5"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
-      <c r="H32" s="1"/>
-      <c r="I32" s="1"/>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A33" s="6"/>
-      <c r="B33" s="7"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="7"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
-      <c r="G33" s="7"/>
-      <c r="H33" s="7"/>
-      <c r="I33" s="7"/>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A34" s="5"/>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
-      <c r="H34" s="1"/>
-      <c r="I34" s="1"/>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A35" s="6"/>
-      <c r="B35" s="7"/>
-      <c r="C35" s="7"/>
-      <c r="D35" s="7"/>
-      <c r="E35" s="7"/>
-      <c r="F35" s="7"/>
-      <c r="G35" s="7"/>
-      <c r="H35" s="7"/>
-      <c r="I35" s="7"/>
+      <c r="A31" s="6"/>
+      <c r="B31" s="7"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="7"/>
+      <c r="H31" s="7"/>
+      <c r="I31" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1902,7 +1571,7 @@
   <dimension ref="A1:V44"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A45" sqref="A45:K50"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2345,7 +2014,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="1">
-        <v>2.0499999999999998</v>
+        <v>2.1</v>
       </c>
       <c r="C15" s="1">
         <v>26.5</v>
@@ -2375,7 +2044,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="1">
-        <v>2.0499999999999998</v>
+        <v>2.1</v>
       </c>
       <c r="C16" s="1">
         <v>177.5</v>
@@ -2992,7 +2661,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P6" sqref="P6"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3125,7 +2794,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1">
-        <v>2.0499999999999998</v>
+        <v>2.1</v>
       </c>
       <c r="C6" s="1">
         <v>2.8</v>
@@ -3194,9 +2863,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3417,27 +3089,15 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44668820-0664-4E62-A660-376AF03334EF}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9421959D-9476-4FEC-BDFE-1367083D3EBE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="f6191221-55a2-427d-afce-6bfcc029a585"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="b60d6f15-5eb1-4c0b-bb71-d899d3bf026f"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3462,9 +3122,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9421959D-9476-4FEC-BDFE-1367083D3EBE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{44668820-0664-4E62-A660-376AF03334EF}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="f6191221-55a2-427d-afce-6bfcc029a585"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="b60d6f15-5eb1-4c0b-bb71-d899d3bf026f"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>